<commit_message>
Update dimensional modelling Workbook - Excel.xlsx
</commit_message>
<xml_diff>
--- a/dimensional modelling Workbook - Excel.xlsx
+++ b/dimensional modelling Workbook - Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\Desktop\cours\NHL-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{770DCDC4-ECC5-4AC0-BE2D-E6F5A27FF8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C1295E-448D-4364-A13E-984F7BB1523D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BusMatrix-HighLevelEntites" sheetId="2" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10818" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10857" uniqueCount="319">
   <si>
     <t>Business Process</t>
   </si>
@@ -1288,13 +1288,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1313,6 +1306,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1533,10 +1533,10 @@
     <tabColor rgb="FF0C343D"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="A1:N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1545,7 +1545,7 @@
     <col min="2" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="123">
+    <row r="1" spans="1:15" ht="123">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1553,43 +1553,46 @@
         <v>302</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="62.25" customHeight="1">
+    <row r="2" spans="1:15" ht="62.25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>297</v>
       </c>
@@ -1599,16 +1602,16 @@
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="6" t="s">
@@ -1617,77 +1620,78 @@
       <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="1:14" ht="62.25" customHeight="1">
+      <c r="L2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="62.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="6"/>
+      <c r="N3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="4" spans="1:14" ht="62.25" customHeight="1">
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" ht="62.25" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="M4" s="6"/>
+      <c r="N4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" ht="62.25" customHeight="1">
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" ht="62.25" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>299</v>
       </c>
@@ -1697,37 +1701,186 @@
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="6"/>
+      <c r="O5" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" ht="15.75" customHeight="1">
+      <c r="C19" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" ht="15.75" customHeight="1">
+      <c r="C20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" ht="15.75" customHeight="1">
+      <c r="C21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="3:14" ht="15.75" customHeight="1">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="3:14" ht="15.75" customHeight="1">
+      <c r="C23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1767,23 +1920,23 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="30"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="J1" s="61" t="s">
         <v>252</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16">
@@ -6792,23 +6945,23 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="30"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="J1" s="61" t="s">
         <v>252</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16">
@@ -16076,20 +16229,20 @@
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="52" t="s">
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
     </row>
     <row r="2" spans="2:18">
       <c r="B2" s="18" t="s">
@@ -23986,7 +24139,7 @@
   </sheetPr>
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -24059,15 +24212,15 @@
       <c r="T1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
     </row>
     <row r="2" spans="1:29" ht="72" customHeight="1">
       <c r="A2" s="9" t="s">
@@ -24122,15 +24275,15 @@
       <c r="T2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="59"/>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="57"/>
-      <c r="AC2" s="57"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
     </row>
     <row r="3" spans="1:29" ht="72" customHeight="1">
       <c r="A3" s="9" t="s">
@@ -24177,15 +24330,15 @@
       <c r="T3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59"/>
-      <c r="Y3" s="59"/>
-      <c r="Z3" s="59"/>
-      <c r="AA3" s="59"/>
-      <c r="AB3" s="57"/>
-      <c r="AC3" s="57"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="54"/>
     </row>
     <row r="4" spans="1:29" ht="72" customHeight="1">
       <c r="A4" s="9" t="s">
@@ -24238,15 +24391,15 @@
       <c r="T4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="59"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="59"/>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="57"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="56"/>
+      <c r="AB4" s="54"/>
+      <c r="AC4" s="54"/>
     </row>
     <row r="5" spans="1:29" ht="72" customHeight="1">
       <c r="A5" s="9" t="s">
@@ -24309,235 +24462,235 @@
       <c r="T5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="U5" s="59"/>
-      <c r="V5" s="59"/>
-      <c r="W5" s="59"/>
-      <c r="X5" s="59"/>
-      <c r="Y5" s="59"/>
-      <c r="Z5" s="59"/>
-      <c r="AA5" s="59"/>
-      <c r="AB5" s="57"/>
-      <c r="AC5" s="57"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56"/>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="56"/>
+      <c r="Z5" s="56"/>
+      <c r="AA5" s="56"/>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="54"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A7" s="57"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A8" s="57"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57"/>
-      <c r="O8" s="57"/>
-      <c r="P8" s="57"/>
-      <c r="Q8" s="57"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="57"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="56"/>
-      <c r="O9" s="57"/>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A10" s="58"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="57"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="57"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A11" s="58"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
+      <c r="T11" s="54"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A12" s="58"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="57"/>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="54"/>
+      <c r="T12" s="54"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A13" s="58"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="57"/>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="54"/>
+      <c r="T13" s="54"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="61"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54"/>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="61"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="54"/>
+      <c r="T15" s="54"/>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="57"/>
-      <c r="S16" s="57"/>
-      <c r="T16" s="57"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="54"/>
+      <c r="T16" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24571,22 +24724,22 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="10"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="59" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="H1" s="54" t="s">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="H1" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
       <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15">
@@ -31170,23 +31323,23 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="10"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="J1" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16">
@@ -41069,23 +41222,23 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="30"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="J1" s="61" t="s">
         <v>245</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16">
@@ -43623,24 +43776,24 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="30"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
       <c r="I1" s="25"/>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="61" t="s">
         <v>245</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16">
@@ -50348,23 +50501,23 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="30"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="J1" s="61" t="s">
         <v>245</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16">
@@ -56997,23 +57150,23 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="30"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="J1" s="61" t="s">
         <v>252</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16">

</xml_diff>